<commit_message>
Data extraction and cleaning completed
</commit_message>
<xml_diff>
--- a/Clean/bridges.xlsx
+++ b/Clean/bridges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\MarABass\Clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9133AB42-B4A3-4453-B2C8-C7E8B31016B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91D12C3-94C1-4587-A71B-4A4711B7D985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -231,17 +231,17 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -566,7 +566,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>